<commit_message>
Maya White blocking updated
</commit_message>
<xml_diff>
--- a/Project 1 Research/Asset List.xlsx
+++ b/Project 1 Research/Asset List.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kand8\Documents\School 19-20\Game Essentials\2221Fall2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10847775\Documents\Game Essentials\2221Fall2019\Project 1 Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F813F40-6E3B-4E9D-A7F7-91473BA1CE49}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{51BDC0AD-FE0A-4B87-AD47-61054E1C1A71}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -329,8 +328,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -350,6 +349,13 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="0.59999389629810485"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -420,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -438,6 +444,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,24 +759,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{284ABF89-08ED-4E05-AF47-E7886A4DF90E}">
-  <dimension ref="A1:F36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="29.5546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" style="5" customWidth="1"/>
     <col min="6" max="6" width="29" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -782,7 +790,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -802,7 +810,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -822,7 +830,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -842,7 +850,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -862,7 +870,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -880,7 +888,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -897,7 +905,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -915,7 +923,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -929,7 +937,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -941,7 +949,7 @@
       <c r="E11" s="13"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -952,7 +960,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
@@ -966,7 +974,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -977,7 +985,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
@@ -989,7 +997,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -997,7 +1005,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -1009,7 +1017,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1017,7 +1025,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
@@ -1027,7 +1035,7 @@
       <c r="E19" s="13"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1035,7 +1043,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
@@ -1047,7 +1055,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1055,7 +1063,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
@@ -1067,12 +1075,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>23</v>
       </c>
@@ -1084,7 +1092,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1092,7 +1100,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>25</v>
       </c>
@@ -1104,7 +1112,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1112,7 +1120,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>27</v>
       </c>
@@ -1124,12 +1132,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>29</v>
       </c>
@@ -1141,7 +1149,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1149,7 +1157,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>31</v>
       </c>
@@ -1159,12 +1167,12 @@
       <c r="E33" s="13"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>33</v>
       </c>
@@ -1174,10 +1182,16 @@
       <c r="E35" s="13"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Asset List Update, missle White Box add
</commit_message>
<xml_diff>
--- a/Project 1 Research/Asset List.xlsx
+++ b/Project 1 Research/Asset List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kand8\Documents\School 19-20\Game Essentials\2221Fall2019\Project 1 Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A14E1A-56C7-4F22-A450-DA29E9B0FC59}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B78272-3FF7-4743-8EBA-7DAABB45CC90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -329,9 +329,6 @@
     <t>LIGHTING</t>
   </si>
   <si>
-    <t>White Blocking</t>
-  </si>
-  <si>
     <t>Modeling</t>
   </si>
   <si>
@@ -354,6 +351,9 @@
   </si>
   <si>
     <t>Texturing</t>
+  </si>
+  <si>
+    <t>White Boxing</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C5700"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -444,7 +444,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -502,8 +502,8 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -818,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61:C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -839,33 +839,33 @@
         <v>90</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>95</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>91</v>
       </c>
       <c r="G1" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>99</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -878,11 +878,12 @@
         <v>1</v>
       </c>
       <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
       <c r="F4" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -890,17 +891,19 @@
         <v>2</v>
       </c>
       <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
       <c r="F6" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -908,14 +911,15 @@
         <v>4</v>
       </c>
       <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
       <c r="E7" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -923,14 +927,15 @@
         <v>5</v>
       </c>
       <c r="B8" s="15"/>
+      <c r="C8" s="16"/>
       <c r="E8" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -938,16 +943,17 @@
         <v>6</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>101</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C9" s="16"/>
       <c r="E9" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -955,16 +961,17 @@
         <v>7</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>101</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C10" s="16"/>
       <c r="E10" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -972,10 +979,11 @@
         <v>8</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>101</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C11" s="16"/>
       <c r="E11" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -983,81 +991,91 @@
         <v>9</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>101</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C12" s="16"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="15"/>
+      <c r="C13" s="16"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>101</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>101</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C15" s="16"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>101</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C16" s="16"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>101</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C17" s="16"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>101</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C18" s="16"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>101</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C19" s="16"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>101</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C20" s="16"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
       <c r="F21" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1065,13 +1083,14 @@
         <v>18</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>101</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C22" s="16"/>
       <c r="F22" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1079,13 +1098,14 @@
         <v>20</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>101</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C23" s="16"/>
       <c r="F23" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1093,13 +1113,14 @@
         <v>21</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>101</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C24" s="16"/>
       <c r="F24" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1107,14 +1128,15 @@
         <v>22</v>
       </c>
       <c r="B25" s="15"/>
+      <c r="C25" s="16"/>
       <c r="E25" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1122,14 +1144,15 @@
         <v>23</v>
       </c>
       <c r="B26" s="15"/>
+      <c r="C26" s="16"/>
       <c r="E26" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1137,14 +1160,15 @@
         <v>24</v>
       </c>
       <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
       <c r="E27" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1152,14 +1176,15 @@
         <v>25</v>
       </c>
       <c r="B28" s="15"/>
+      <c r="C28" s="16"/>
       <c r="E28" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1167,14 +1192,15 @@
         <v>26</v>
       </c>
       <c r="B29" s="15"/>
+      <c r="C29" s="16"/>
       <c r="E29" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -1182,14 +1208,15 @@
         <v>27</v>
       </c>
       <c r="B30" s="15"/>
+      <c r="C30" s="16"/>
       <c r="E30" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -1197,14 +1224,15 @@
         <v>28</v>
       </c>
       <c r="B31" s="15"/>
+      <c r="C31" s="16"/>
       <c r="E31" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1212,14 +1240,15 @@
         <v>29</v>
       </c>
       <c r="B32" s="15"/>
+      <c r="C32" s="16"/>
       <c r="E32" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -1227,14 +1256,15 @@
         <v>30</v>
       </c>
       <c r="B33" s="15"/>
+      <c r="C33" s="16"/>
       <c r="E33" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -1242,11 +1272,12 @@
         <v>31</v>
       </c>
       <c r="B34" s="15"/>
+      <c r="C34" s="16"/>
       <c r="E34" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -1254,13 +1285,14 @@
         <v>32</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>101</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C35" s="16"/>
       <c r="E35" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G35" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -1268,14 +1300,15 @@
         <v>35</v>
       </c>
       <c r="B36" s="15"/>
+      <c r="C36" s="16"/>
       <c r="E36" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G36" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -1291,14 +1324,15 @@
         <v>37</v>
       </c>
       <c r="B39" s="15"/>
+      <c r="C39" s="16"/>
       <c r="E39" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G39" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -1306,14 +1340,15 @@
         <v>38</v>
       </c>
       <c r="B40" s="15"/>
+      <c r="C40" s="16"/>
       <c r="E40" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G40" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -1321,14 +1356,15 @@
         <v>40</v>
       </c>
       <c r="B41" s="15"/>
+      <c r="C41" s="16"/>
       <c r="E41" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G41" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -1336,16 +1372,17 @@
         <v>39</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>101</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C42" s="16"/>
       <c r="E42" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -1353,13 +1390,14 @@
         <v>33</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>101</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C43" s="16"/>
       <c r="E43" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G43" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -1367,13 +1405,14 @@
         <v>34</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>101</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C44" s="16"/>
       <c r="E44" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G44" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -1381,14 +1420,15 @@
         <v>41</v>
       </c>
       <c r="B45" s="15"/>
+      <c r="C45" s="16"/>
       <c r="E45" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G45" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -1396,14 +1436,15 @@
         <v>42</v>
       </c>
       <c r="B46" s="15"/>
+      <c r="C46" s="16"/>
       <c r="E46" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G46" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -1411,14 +1452,15 @@
         <v>43</v>
       </c>
       <c r="B47" s="15"/>
+      <c r="C47" s="16"/>
       <c r="E47" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G47" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -1426,14 +1468,15 @@
         <v>44</v>
       </c>
       <c r="B48" s="15"/>
+      <c r="C48" s="16"/>
       <c r="E48" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G48" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -1441,14 +1484,15 @@
         <v>45</v>
       </c>
       <c r="B49" s="15"/>
+      <c r="C49" s="16"/>
       <c r="E49" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G49" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -1461,14 +1505,15 @@
         <v>49</v>
       </c>
       <c r="B52" s="15"/>
+      <c r="C52" s="16"/>
       <c r="E52" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F52" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G52" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -1476,14 +1521,15 @@
         <v>47</v>
       </c>
       <c r="B53" s="15"/>
+      <c r="C53" s="16"/>
       <c r="E53" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G53" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -1491,14 +1537,15 @@
         <v>48</v>
       </c>
       <c r="B54" s="15"/>
+      <c r="C54" s="16"/>
       <c r="E54" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G54" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -1506,14 +1553,15 @@
         <v>50</v>
       </c>
       <c r="B55" s="15"/>
+      <c r="C55" s="16"/>
       <c r="E55" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G55" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
@@ -1521,14 +1569,15 @@
         <v>51</v>
       </c>
       <c r="B56" s="15"/>
+      <c r="C56" s="16"/>
       <c r="E56" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G56" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
@@ -1536,14 +1585,15 @@
         <v>52</v>
       </c>
       <c r="B57" s="15"/>
+      <c r="C57" s="16"/>
       <c r="E57" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G57" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -1551,16 +1601,17 @@
         <v>53</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>101</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C58" s="16"/>
       <c r="E58" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F58" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G58" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
@@ -1572,22 +1623,25 @@
       <c r="A61" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B61" s="16"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="16"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B62" s="16"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="16"/>
       <c r="D62" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B63" s="16"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="16"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
@@ -1604,16 +1658,16 @@
         <v>59</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E67" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -1622,13 +1676,13 @@
       </c>
       <c r="B68" s="15"/>
       <c r="C68" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E68" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -1636,16 +1690,16 @@
         <v>61</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E69" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -1653,16 +1707,16 @@
         <v>62</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E70" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -1670,16 +1724,16 @@
         <v>63</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E71" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
@@ -1687,16 +1741,16 @@
         <v>64</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E72" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -1704,16 +1758,16 @@
         <v>65</v>
       </c>
       <c r="B73" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E73" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
@@ -1736,16 +1790,16 @@
         <v>68</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E77" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
@@ -1753,16 +1807,16 @@
         <v>67</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E78" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -1770,16 +1824,16 @@
         <v>69</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E79" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -1787,16 +1841,16 @@
         <v>70</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E80" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -1804,16 +1858,16 @@
         <v>71</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E81" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -1821,16 +1875,16 @@
         <v>72</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E82" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -1847,19 +1901,19 @@
         <v>74</v>
       </c>
       <c r="B85" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E85" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -1867,19 +1921,19 @@
         <v>75</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C86" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E86" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F86" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -1887,19 +1941,19 @@
         <v>76</v>
       </c>
       <c r="B87" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E87" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F87" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -1907,19 +1961,19 @@
         <v>77</v>
       </c>
       <c r="B88" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E88" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F88" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -1927,19 +1981,19 @@
         <v>78</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C89" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E89" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F89" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -1947,19 +2001,19 @@
         <v>79</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C90" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D90" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E90" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F90" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -1976,13 +2030,13 @@
         <v>81</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C93" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D93" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -1990,13 +2044,13 @@
         <v>82</v>
       </c>
       <c r="B94" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -2004,13 +2058,13 @@
         <v>83</v>
       </c>
       <c r="B95" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C95" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -2027,13 +2081,13 @@
         <v>85</v>
       </c>
       <c r="B98" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -2041,13 +2095,13 @@
         <v>86</v>
       </c>
       <c r="B99" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C99" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -2055,13 +2109,13 @@
         <v>66</v>
       </c>
       <c r="B100" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -2069,13 +2123,13 @@
         <v>87</v>
       </c>
       <c r="B101" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -2092,16 +2146,16 @@
         <v>89</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C104" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D104" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F104" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>